<commit_message>
Added new bom, LPC Dev Board
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="239">
   <si>
     <t>Comment</t>
   </si>
@@ -732,6 +732,15 @@
   </si>
   <si>
     <t>ERJ-6GEYJ270V</t>
+  </si>
+  <si>
+    <t>RTC backup cap</t>
+  </si>
+  <si>
+    <t>11mF</t>
+  </si>
+  <si>
+    <t>CPH3225A</t>
   </si>
 </sst>
 </file>
@@ -829,7 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,6 +854,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1160,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,7 +1297,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>24</v>
@@ -1790,7 +1800,7 @@
         <v>30</v>
       </c>
       <c r="G21" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>217</v>
@@ -1866,7 +1876,7 @@
         <v>30</v>
       </c>
       <c r="G24" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>218</v>
@@ -1896,7 +1906,7 @@
         <v>130</v>
       </c>
       <c r="G25" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>130</v>
@@ -2170,7 +2180,7 @@
         <v>174</v>
       </c>
       <c r="G35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>174</v>
@@ -2439,6 +2449,24 @@
         <v>Digikey - P0.0ACT-ND</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I47" s="6" t="str">
+        <f>HYPERLINK("http://www.digikey.ca/product-detail/en/seiko-instruments/CPH3225A/728-1067-1-ND/4747400","Digikey - 728-1067-1-ND")</f>
+        <v>Digikey - 728-1067-1-ND</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>